<commit_message>
Extended the verification and PoK phases
</commit_message>
<xml_diff>
--- a/Result1.xlsx
+++ b/Result1.xlsx
@@ -504,13 +504,13 @@
         <v>100</v>
       </c>
       <c r="D2" t="n">
-        <v>0.32463</v>
+        <v>0.53849</v>
       </c>
       <c r="E2" t="n">
-        <v>876</v>
+        <v>1390</v>
       </c>
       <c r="F2" t="n">
-        <v>0.20274</v>
+        <v>0.21302</v>
       </c>
       <c r="G2" t="n">
         <v>20</v>
@@ -519,22 +519,22 @@
         <v>10.1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.07132000000000001</v>
+        <v>0.06018</v>
       </c>
       <c r="J2" t="n">
         <v>14.4</v>
       </c>
       <c r="K2" t="n">
-        <v>2.06453</v>
+        <v>2.08018</v>
       </c>
       <c r="L2" t="n">
         <v>1258</v>
       </c>
       <c r="M2" t="n">
-        <v>1.67518</v>
+        <v>1.88554</v>
       </c>
       <c r="N2" t="n">
-        <v>0.00204</v>
+        <v>0.00101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved the overhead of verification
</commit_message>
<xml_diff>
--- a/Result1.xlsx
+++ b/Result1.xlsx
@@ -504,13 +504,13 @@
         <v>100</v>
       </c>
       <c r="D2" t="n">
-        <v>0.53849</v>
+        <v>0.53611</v>
       </c>
       <c r="E2" t="n">
         <v>1390</v>
       </c>
       <c r="F2" t="n">
-        <v>0.21302</v>
+        <v>0.20778</v>
       </c>
       <c r="G2" t="n">
         <v>20</v>
@@ -519,22 +519,22 @@
         <v>10.1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.06018</v>
+        <v>0.06054999999999999</v>
       </c>
       <c r="J2" t="n">
         <v>14.4</v>
       </c>
       <c r="K2" t="n">
-        <v>2.08018</v>
+        <v>1.99466</v>
       </c>
       <c r="L2" t="n">
         <v>1258</v>
       </c>
       <c r="M2" t="n">
-        <v>1.88554</v>
+        <v>1.88371</v>
       </c>
       <c r="N2" t="n">
-        <v>0.00101</v>
+        <v>0.00124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding the new results
</commit_message>
<xml_diff>
--- a/Result1.xlsx
+++ b/Result1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,46 +495,1278 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>50</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.050425</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.01114</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.002966</v>
+      </c>
+      <c r="J2" t="n">
+        <v>14</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.15205</v>
+      </c>
+      <c r="L2" t="n">
+        <v>5554</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.172362</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.000148</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C3" t="n">
         <v>100</v>
       </c>
-      <c r="D2" t="n">
-        <v>0.53611</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1390</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.20778</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="D3" t="n">
+        <v>0.052951</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.019302</v>
+      </c>
+      <c r="G3" t="n">
         <v>20</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H3" t="n">
         <v>10.1</v>
       </c>
-      <c r="I2" t="n">
-        <v>0.06054999999999999</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="I3" t="n">
+        <v>0.005628</v>
+      </c>
+      <c r="J3" t="n">
         <v>14.4</v>
       </c>
-      <c r="K2" t="n">
-        <v>1.99466</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1258</v>
-      </c>
-      <c r="M2" t="n">
-        <v>1.88371</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.00124</v>
+      <c r="K3" t="n">
+        <v>0.187161</v>
+      </c>
+      <c r="L3" t="n">
+        <v>5556</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.179755</v>
+      </c>
+      <c r="N3" t="n">
+        <v>5.3e-05</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>150</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.054525</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.027286</v>
+      </c>
+      <c r="G4" t="n">
+        <v>30</v>
+      </c>
+      <c r="H4" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.007649</v>
+      </c>
+      <c r="J4" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.226148</v>
+      </c>
+      <c r="L4" t="n">
+        <v>5558</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.189559</v>
+      </c>
+      <c r="N4" t="n">
+        <v>6.2e-05</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>200</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.053915</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.035076</v>
+      </c>
+      <c r="G5" t="n">
+        <v>40</v>
+      </c>
+      <c r="H5" t="n">
+        <v>20.1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.009945000000000001</v>
+      </c>
+      <c r="J5" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.263796</v>
+      </c>
+      <c r="L5" t="n">
+        <v>5560</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.199391</v>
+      </c>
+      <c r="N5" t="n">
+        <v>5.8e-05</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>250</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.053569</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.043516</v>
+      </c>
+      <c r="G6" t="n">
+        <v>50</v>
+      </c>
+      <c r="H6" t="n">
+        <v>25.1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.012363</v>
+      </c>
+      <c r="J6" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.30159</v>
+      </c>
+      <c r="L6" t="n">
+        <v>5562</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.20926</v>
+      </c>
+      <c r="N6" t="n">
+        <v>5.8e-05</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>300</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.054827</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.052224</v>
+      </c>
+      <c r="G7" t="n">
+        <v>60</v>
+      </c>
+      <c r="H7" t="n">
+        <v>30.1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.014951</v>
+      </c>
+      <c r="J7" t="n">
+        <v>16</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.338832</v>
+      </c>
+      <c r="L7" t="n">
+        <v>5564</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.219167</v>
+      </c>
+      <c r="N7" t="n">
+        <v>6.1e-05</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>350</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.054204</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.06052</v>
+      </c>
+      <c r="G8" t="n">
+        <v>70</v>
+      </c>
+      <c r="H8" t="n">
+        <v>35.1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.017448</v>
+      </c>
+      <c r="J8" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.37759</v>
+      </c>
+      <c r="L8" t="n">
+        <v>5566</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.22544</v>
+      </c>
+      <c r="N8" t="n">
+        <v>5.7e-05</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>400</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.053601</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.069054</v>
+      </c>
+      <c r="G9" t="n">
+        <v>80</v>
+      </c>
+      <c r="H9" t="n">
+        <v>40.1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.019735</v>
+      </c>
+      <c r="J9" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.414003</v>
+      </c>
+      <c r="L9" t="n">
+        <v>5568</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.235362</v>
+      </c>
+      <c r="N9" t="n">
+        <v>5.7e-05</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>450</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.054492</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.077627</v>
+      </c>
+      <c r="G10" t="n">
+        <v>90</v>
+      </c>
+      <c r="H10" t="n">
+        <v>45.1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.02287</v>
+      </c>
+      <c r="J10" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.452297</v>
+      </c>
+      <c r="L10" t="n">
+        <v>5570</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.246277</v>
+      </c>
+      <c r="N10" t="n">
+        <v>5.7e-05</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>500</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.054119</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.08592</v>
+      </c>
+      <c r="G11" t="n">
+        <v>100</v>
+      </c>
+      <c r="H11" t="n">
+        <v>50.1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.024983</v>
+      </c>
+      <c r="J11" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.489629</v>
+      </c>
+      <c r="L11" t="n">
+        <v>5572</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.255794</v>
+      </c>
+      <c r="N11" t="n">
+        <v>6.600000000000001e-05</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>550</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.053712</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.09400600000000001</v>
+      </c>
+      <c r="G12" t="n">
+        <v>110</v>
+      </c>
+      <c r="H12" t="n">
+        <v>55.1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.02686</v>
+      </c>
+      <c r="J12" t="n">
+        <v>18</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.527228</v>
+      </c>
+      <c r="L12" t="n">
+        <v>5574</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.263933</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.000109</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="n">
+        <v>600</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.054303</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.102987</v>
+      </c>
+      <c r="G13" t="n">
+        <v>120</v>
+      </c>
+      <c r="H13" t="n">
+        <v>60.1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.029186</v>
+      </c>
+      <c r="J13" t="n">
+        <v>18.4</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.56447</v>
+      </c>
+      <c r="L13" t="n">
+        <v>5576</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.272043</v>
+      </c>
+      <c r="N13" t="n">
+        <v>6.4e-05</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="n">
+        <v>650</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.053443</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.111902</v>
+      </c>
+      <c r="G14" t="n">
+        <v>130</v>
+      </c>
+      <c r="H14" t="n">
+        <v>65.09999999999999</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.031828</v>
+      </c>
+      <c r="J14" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.598623</v>
+      </c>
+      <c r="L14" t="n">
+        <v>5578</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.279054</v>
+      </c>
+      <c r="N14" t="n">
+        <v>7.1e-05</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="n">
+        <v>700</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.056002</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.12056</v>
+      </c>
+      <c r="G15" t="n">
+        <v>140</v>
+      </c>
+      <c r="H15" t="n">
+        <v>70.09999999999999</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.034123</v>
+      </c>
+      <c r="J15" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.632675</v>
+      </c>
+      <c r="L15" t="n">
+        <v>5580</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.28924</v>
+      </c>
+      <c r="N15" t="n">
+        <v>7.499999999999999e-05</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="n">
+        <v>750</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.053054</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.127663</v>
+      </c>
+      <c r="G16" t="n">
+        <v>150</v>
+      </c>
+      <c r="H16" t="n">
+        <v>75.09999999999999</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.035978</v>
+      </c>
+      <c r="J16" t="n">
+        <v>19.6</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.669941</v>
+      </c>
+      <c r="L16" t="n">
+        <v>5582</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.297546</v>
+      </c>
+      <c r="N16" t="n">
+        <v>6.8e-05</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="n">
+        <v>800</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.054469</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.135853</v>
+      </c>
+      <c r="G17" t="n">
+        <v>160</v>
+      </c>
+      <c r="H17" t="n">
+        <v>80.09999999999999</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.038693</v>
+      </c>
+      <c r="J17" t="n">
+        <v>20</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.705227</v>
+      </c>
+      <c r="L17" t="n">
+        <v>5584</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.305146</v>
+      </c>
+      <c r="N17" t="n">
+        <v>6.600000000000001e-05</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" t="n">
+        <v>850</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.054111</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.143593</v>
+      </c>
+      <c r="G18" t="n">
+        <v>170</v>
+      </c>
+      <c r="H18" t="n">
+        <v>85.09999999999999</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.03996</v>
+      </c>
+      <c r="J18" t="n">
+        <v>20.4</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.743545</v>
+      </c>
+      <c r="L18" t="n">
+        <v>5586</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.315617</v>
+      </c>
+      <c r="N18" t="n">
+        <v>7.4e-05</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" t="n">
+        <v>900</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.054157</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.154444</v>
+      </c>
+      <c r="G19" t="n">
+        <v>180</v>
+      </c>
+      <c r="H19" t="n">
+        <v>90.09999999999999</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.043219</v>
+      </c>
+      <c r="J19" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.7792559999999999</v>
+      </c>
+      <c r="L19" t="n">
+        <v>5588</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.323774</v>
+      </c>
+      <c r="N19" t="n">
+        <v>6.7e-05</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>19</v>
+      </c>
+      <c r="C20" t="n">
+        <v>950</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.053809</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.16055</v>
+      </c>
+      <c r="G20" t="n">
+        <v>190</v>
+      </c>
+      <c r="H20" t="n">
+        <v>95.09999999999999</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.045074</v>
+      </c>
+      <c r="J20" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.812842</v>
+      </c>
+      <c r="L20" t="n">
+        <v>5590</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.33307</v>
+      </c>
+      <c r="N20" t="n">
+        <v>7.7e-05</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.055265</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.172566</v>
+      </c>
+      <c r="G21" t="n">
+        <v>200</v>
+      </c>
+      <c r="H21" t="n">
+        <v>100.1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.046344</v>
+      </c>
+      <c r="J21" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.849146</v>
+      </c>
+      <c r="L21" t="n">
+        <v>5592</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.341354</v>
+      </c>
+      <c r="N21" t="n">
+        <v>6.999999999999999e-05</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1050</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.056827</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.180252</v>
+      </c>
+      <c r="G22" t="n">
+        <v>210</v>
+      </c>
+      <c r="H22" t="n">
+        <v>105.1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.052093</v>
+      </c>
+      <c r="J22" t="n">
+        <v>22</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.8844340000000001</v>
+      </c>
+      <c r="L22" t="n">
+        <v>5594</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.34961</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.000127</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>22</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1100</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.061529</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.19318</v>
+      </c>
+      <c r="G23" t="n">
+        <v>220</v>
+      </c>
+      <c r="H23" t="n">
+        <v>110.1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.05709</v>
+      </c>
+      <c r="J23" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.982032</v>
+      </c>
+      <c r="L23" t="n">
+        <v>5596</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.378613</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.000105</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1150</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.057594</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.197185</v>
+      </c>
+      <c r="G24" t="n">
+        <v>230</v>
+      </c>
+      <c r="H24" t="n">
+        <v>115.1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.054939</v>
+      </c>
+      <c r="J24" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.955493</v>
+      </c>
+      <c r="L24" t="n">
+        <v>5598</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.365707</v>
+      </c>
+      <c r="N24" t="n">
+        <v>7.1e-05</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.056834</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.205761</v>
+      </c>
+      <c r="G25" t="n">
+        <v>240</v>
+      </c>
+      <c r="H25" t="n">
+        <v>120.1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.0565</v>
+      </c>
+      <c r="J25" t="n">
+        <v>23.2</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1.004384</v>
+      </c>
+      <c r="L25" t="n">
+        <v>5600</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.384931</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.000117</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>25</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1250</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.057701</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.214577</v>
+      </c>
+      <c r="G26" t="n">
+        <v>250</v>
+      </c>
+      <c r="H26" t="n">
+        <v>125.1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.061494</v>
+      </c>
+      <c r="J26" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1.055081</v>
+      </c>
+      <c r="L26" t="n">
+        <v>5602</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.393284</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.00014</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>26</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.058032</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.223738</v>
+      </c>
+      <c r="G27" t="n">
+        <v>260</v>
+      </c>
+      <c r="H27" t="n">
+        <v>130.1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.06371300000000001</v>
+      </c>
+      <c r="J27" t="n">
+        <v>24</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1.09012</v>
+      </c>
+      <c r="L27" t="n">
+        <v>5604</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.402774</v>
+      </c>
+      <c r="N27" t="n">
+        <v>8.8e-05</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>27</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1350</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.066883</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.238558</v>
+      </c>
+      <c r="G28" t="n">
+        <v>270</v>
+      </c>
+      <c r="H28" t="n">
+        <v>135.1</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.064997</v>
+      </c>
+      <c r="J28" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1.172569</v>
+      </c>
+      <c r="L28" t="n">
+        <v>5606</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.420699</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.000144</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>28</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1400</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.058049</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.241472</v>
+      </c>
+      <c r="G29" t="n">
+        <v>280</v>
+      </c>
+      <c r="H29" t="n">
+        <v>140.1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.068236</v>
+      </c>
+      <c r="J29" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1.162706</v>
+      </c>
+      <c r="L29" t="n">
+        <v>5608</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.418973</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.000138</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>29</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1450</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.06281299999999999</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.24828</v>
+      </c>
+      <c r="G30" t="n">
+        <v>290</v>
+      </c>
+      <c r="H30" t="n">
+        <v>145.1</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.070868</v>
+      </c>
+      <c r="J30" t="n">
+        <v>25.2</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1.197927</v>
+      </c>
+      <c r="L30" t="n">
+        <v>5610</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.432606</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.000139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated some parts of the code
</commit_message>
<xml_diff>
--- a/Result1.xlsx
+++ b/Result1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,13 +509,13 @@
         <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>0.06965499999999999</v>
+        <v>0.052549</v>
       </c>
       <c r="E2" t="n">
         <v>1390</v>
       </c>
       <c r="F2" t="n">
-        <v>11.2369</v>
+        <v>9.545200000000001</v>
       </c>
       <c r="G2" t="n">
         <v>10</v>
@@ -524,25 +524,1858 @@
         <v>5.1</v>
       </c>
       <c r="I2" t="n">
-        <v>3.0077</v>
+        <v>2.926</v>
       </c>
       <c r="J2" t="n">
         <v>140</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1691464</v>
+        <v>0.1537627</v>
       </c>
       <c r="L2" t="n">
         <v>5.554</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1416848</v>
+        <v>0.1254568</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1884608</v>
+        <v>0.1736193</v>
       </c>
       <c r="O2" t="n">
-        <v>0.000145</v>
+        <v>0.000123</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.054139</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F3" t="n">
+        <v>18.6972</v>
+      </c>
+      <c r="G3" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>5.433399999999999</v>
+      </c>
+      <c r="J3" t="n">
+        <v>144</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.1928538</v>
+      </c>
+      <c r="L3" t="n">
+        <v>5.556</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.1398514</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.1840445</v>
+      </c>
+      <c r="O3" t="n">
+        <v>6.3e-05</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>150</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.053693</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F4" t="n">
+        <v>28.3824</v>
+      </c>
+      <c r="G4" t="n">
+        <v>30</v>
+      </c>
+      <c r="H4" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>7.903199999999999</v>
+      </c>
+      <c r="J4" t="n">
+        <v>148</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.2305282</v>
+      </c>
+      <c r="L4" t="n">
+        <v>5.558</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.1540413</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.1931213</v>
+      </c>
+      <c r="O4" t="n">
+        <v>6.4e-05</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>200</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.054812</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F5" t="n">
+        <v>37.36190000000001</v>
+      </c>
+      <c r="G5" t="n">
+        <v>40</v>
+      </c>
+      <c r="H5" t="n">
+        <v>20.1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>10.9806</v>
+      </c>
+      <c r="J5" t="n">
+        <v>152</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.2902018</v>
+      </c>
+      <c r="L5" t="n">
+        <v>5.56</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.1797343</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.2156712</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.000102</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>250</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.06251</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F6" t="n">
+        <v>45.4171</v>
+      </c>
+      <c r="G6" t="n">
+        <v>50</v>
+      </c>
+      <c r="H6" t="n">
+        <v>25.1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>12.5169</v>
+      </c>
+      <c r="J6" t="n">
+        <v>156</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.299648</v>
+      </c>
+      <c r="L6" t="n">
+        <v>5.562</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.1777948</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.2062082</v>
+      </c>
+      <c r="O6" t="n">
+        <v>7.499999999999999e-05</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>300</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.052979</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F7" t="n">
+        <v>53.5369</v>
+      </c>
+      <c r="G7" t="n">
+        <v>60</v>
+      </c>
+      <c r="H7" t="n">
+        <v>30.1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>14.9292</v>
+      </c>
+      <c r="J7" t="n">
+        <v>160</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.336773</v>
+      </c>
+      <c r="L7" t="n">
+        <v>5.564</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.1919923</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.2162533</v>
+      </c>
+      <c r="O7" t="n">
+        <v>6.4e-05</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>350</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.052902</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F8" t="n">
+        <v>61.62259999999999</v>
+      </c>
+      <c r="G8" t="n">
+        <v>70</v>
+      </c>
+      <c r="H8" t="n">
+        <v>35.1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>17.0428</v>
+      </c>
+      <c r="J8" t="n">
+        <v>164</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.3726058</v>
+      </c>
+      <c r="L8" t="n">
+        <v>5.566</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.2033476</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.2242484</v>
+      </c>
+      <c r="O8" t="n">
+        <v>6.1e-05</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>400</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.055172</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F9" t="n">
+        <v>70.01090000000001</v>
+      </c>
+      <c r="G9" t="n">
+        <v>80</v>
+      </c>
+      <c r="H9" t="n">
+        <v>40.1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>19.5262</v>
+      </c>
+      <c r="J9" t="n">
+        <v>168</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.4096295</v>
+      </c>
+      <c r="L9" t="n">
+        <v>5.568</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.2170965</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.2335689</v>
+      </c>
+      <c r="O9" t="n">
+        <v>6.2e-05</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>450</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.053458</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F10" t="n">
+        <v>78.3741</v>
+      </c>
+      <c r="G10" t="n">
+        <v>90</v>
+      </c>
+      <c r="H10" t="n">
+        <v>45.1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>21.858</v>
+      </c>
+      <c r="J10" t="n">
+        <v>172</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.4437589</v>
+      </c>
+      <c r="L10" t="n">
+        <v>5.57</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.228919</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.2424077000000001</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.000139</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>500</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.055756</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F11" t="n">
+        <v>87.99189999999999</v>
+      </c>
+      <c r="G11" t="n">
+        <v>100</v>
+      </c>
+      <c r="H11" t="n">
+        <v>50.1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>24.3612</v>
+      </c>
+      <c r="J11" t="n">
+        <v>176</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.4895905</v>
+      </c>
+      <c r="L11" t="n">
+        <v>5.572</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.2465309</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.2542703</v>
+      </c>
+      <c r="O11" t="n">
+        <v>6.9e-05</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>550</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.055886</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F12" t="n">
+        <v>97.4396</v>
+      </c>
+      <c r="G12" t="n">
+        <v>110</v>
+      </c>
+      <c r="H12" t="n">
+        <v>55.1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>27.1065</v>
+      </c>
+      <c r="J12" t="n">
+        <v>180</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.5278084</v>
+      </c>
+      <c r="L12" t="n">
+        <v>5.574</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.256859</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.2577896</v>
+      </c>
+      <c r="O12" t="n">
+        <v>6.600000000000001e-05</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="n">
+        <v>600</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.055892</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F13" t="n">
+        <v>104.644</v>
+      </c>
+      <c r="G13" t="n">
+        <v>120</v>
+      </c>
+      <c r="H13" t="n">
+        <v>60.1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>29.788</v>
+      </c>
+      <c r="J13" t="n">
+        <v>184</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.5826648000000001</v>
+      </c>
+      <c r="L13" t="n">
+        <v>5.576</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.2850456</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.2831462</v>
+      </c>
+      <c r="O13" t="n">
+        <v>6.7e-05</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="n">
+        <v>650</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.054517</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F14" t="n">
+        <v>120.2379</v>
+      </c>
+      <c r="G14" t="n">
+        <v>130</v>
+      </c>
+      <c r="H14" t="n">
+        <v>65.09999999999999</v>
+      </c>
+      <c r="I14" t="n">
+        <v>34.5411</v>
+      </c>
+      <c r="J14" t="n">
+        <v>188</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.6049455</v>
+      </c>
+      <c r="L14" t="n">
+        <v>5.578</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.2870220000000001</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.2808252000000001</v>
+      </c>
+      <c r="O14" t="n">
+        <v>6.9e-05</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="n">
+        <v>700</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.054807</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F15" t="n">
+        <v>121.4169</v>
+      </c>
+      <c r="G15" t="n">
+        <v>140</v>
+      </c>
+      <c r="H15" t="n">
+        <v>70.09999999999999</v>
+      </c>
+      <c r="I15" t="n">
+        <v>33.5519</v>
+      </c>
+      <c r="J15" t="n">
+        <v>192</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.6354078</v>
+      </c>
+      <c r="L15" t="n">
+        <v>5.58</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.3000686</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.2899351000000001</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.000114</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="n">
+        <v>750</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.054387</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F16" t="n">
+        <v>129.5623</v>
+      </c>
+      <c r="G16" t="n">
+        <v>150</v>
+      </c>
+      <c r="H16" t="n">
+        <v>75.09999999999999</v>
+      </c>
+      <c r="I16" t="n">
+        <v>36.0524</v>
+      </c>
+      <c r="J16" t="n">
+        <v>196</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.6719547</v>
+      </c>
+      <c r="L16" t="n">
+        <v>5.582</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.3147718</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.2993781</v>
+      </c>
+      <c r="O16" t="n">
+        <v>7.1e-05</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="n">
+        <v>800</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.054603</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F17" t="n">
+        <v>139.3939</v>
+      </c>
+      <c r="G17" t="n">
+        <v>160</v>
+      </c>
+      <c r="H17" t="n">
+        <v>80.09999999999999</v>
+      </c>
+      <c r="I17" t="n">
+        <v>39.3358</v>
+      </c>
+      <c r="J17" t="n">
+        <v>200</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.7370778999999998</v>
+      </c>
+      <c r="L17" t="n">
+        <v>5.584</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.3376879</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.3182576</v>
+      </c>
+      <c r="O17" t="n">
+        <v>7.2e-05</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" t="n">
+        <v>850</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.053937</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F18" t="n">
+        <v>148.8467</v>
+      </c>
+      <c r="G18" t="n">
+        <v>170</v>
+      </c>
+      <c r="H18" t="n">
+        <v>85.09999999999999</v>
+      </c>
+      <c r="I18" t="n">
+        <v>41.5898</v>
+      </c>
+      <c r="J18" t="n">
+        <v>204</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.7706412</v>
+      </c>
+      <c r="L18" t="n">
+        <v>5.586</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.3519054</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.3274354</v>
+      </c>
+      <c r="O18" t="n">
+        <v>7.1e-05</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" t="n">
+        <v>900</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.05507</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F19" t="n">
+        <v>159.2303</v>
+      </c>
+      <c r="G19" t="n">
+        <v>180</v>
+      </c>
+      <c r="H19" t="n">
+        <v>90.09999999999999</v>
+      </c>
+      <c r="I19" t="n">
+        <v>44.1563</v>
+      </c>
+      <c r="J19" t="n">
+        <v>208</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.8124869</v>
+      </c>
+      <c r="L19" t="n">
+        <v>5.588</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.3646759000000001</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.3324665999999999</v>
+      </c>
+      <c r="O19" t="n">
+        <v>7.3e-05</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>19</v>
+      </c>
+      <c r="C20" t="n">
+        <v>950</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.054936</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F20" t="n">
+        <v>165.8284</v>
+      </c>
+      <c r="G20" t="n">
+        <v>190</v>
+      </c>
+      <c r="H20" t="n">
+        <v>95.09999999999999</v>
+      </c>
+      <c r="I20" t="n">
+        <v>46.15519999999999</v>
+      </c>
+      <c r="J20" t="n">
+        <v>212</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.8412602</v>
+      </c>
+      <c r="L20" t="n">
+        <v>5.59</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.3765679</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.3428398</v>
+      </c>
+      <c r="O20" t="n">
+        <v>7.3e-05</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.053709</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F21" t="n">
+        <v>174.1295</v>
+      </c>
+      <c r="G21" t="n">
+        <v>200</v>
+      </c>
+      <c r="H21" t="n">
+        <v>100.1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>48.43899999999999</v>
+      </c>
+      <c r="J21" t="n">
+        <v>216</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.8779028</v>
+      </c>
+      <c r="L21" t="n">
+        <v>5.592</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.3898503</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.3525849</v>
+      </c>
+      <c r="O21" t="n">
+        <v>7.4e-05</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1050</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.054049</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F22" t="n">
+        <v>182.9373</v>
+      </c>
+      <c r="G22" t="n">
+        <v>210</v>
+      </c>
+      <c r="H22" t="n">
+        <v>105.1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>51.3694</v>
+      </c>
+      <c r="J22" t="n">
+        <v>220</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.9187717</v>
+      </c>
+      <c r="L22" t="n">
+        <v>5.594</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.4051508</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.3629322</v>
+      </c>
+      <c r="O22" t="n">
+        <v>7.4e-05</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>22</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1100</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.053611</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F23" t="n">
+        <v>192.7913</v>
+      </c>
+      <c r="G23" t="n">
+        <v>220</v>
+      </c>
+      <c r="H23" t="n">
+        <v>110.1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>53.4738</v>
+      </c>
+      <c r="J23" t="n">
+        <v>224</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.9564698</v>
+      </c>
+      <c r="L23" t="n">
+        <v>5.596</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.4196367</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.3736382</v>
+      </c>
+      <c r="O23" t="n">
+        <v>7.3e-05</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1150</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.053991</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F24" t="n">
+        <v>199.943</v>
+      </c>
+      <c r="G24" t="n">
+        <v>230</v>
+      </c>
+      <c r="H24" t="n">
+        <v>115.1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>56.0547</v>
+      </c>
+      <c r="J24" t="n">
+        <v>228</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.9953750000000001</v>
+      </c>
+      <c r="L24" t="n">
+        <v>5.598</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.418044</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.3661</v>
+      </c>
+      <c r="O24" t="n">
+        <v>6.999999999999999e-05</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.054232</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F25" t="n">
+        <v>202.5211</v>
+      </c>
+      <c r="G25" t="n">
+        <v>240</v>
+      </c>
+      <c r="H25" t="n">
+        <v>120.1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>56.224</v>
+      </c>
+      <c r="J25" t="n">
+        <v>232</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.9816559000000001</v>
+      </c>
+      <c r="L25" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.4256817</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.3721624</v>
+      </c>
+      <c r="O25" t="n">
+        <v>7.4e-05</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>25</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1250</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.055176</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F26" t="n">
+        <v>210.5076</v>
+      </c>
+      <c r="G26" t="n">
+        <v>250</v>
+      </c>
+      <c r="H26" t="n">
+        <v>125.1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>58.4288</v>
+      </c>
+      <c r="J26" t="n">
+        <v>236</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1.0154671</v>
+      </c>
+      <c r="L26" t="n">
+        <v>5.602</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.4407165</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.3819128</v>
+      </c>
+      <c r="O26" t="n">
+        <v>8.6e-05</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>26</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.055335</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F27" t="n">
+        <v>220.9144</v>
+      </c>
+      <c r="G27" t="n">
+        <v>260</v>
+      </c>
+      <c r="H27" t="n">
+        <v>130.1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>61.32240000000001</v>
+      </c>
+      <c r="J27" t="n">
+        <v>240</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1.0511457</v>
+      </c>
+      <c r="L27" t="n">
+        <v>5.604</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.4486199</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.3870955</v>
+      </c>
+      <c r="O27" t="n">
+        <v>7.6e-05</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>27</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1350</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.053211</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F28" t="n">
+        <v>226.1527</v>
+      </c>
+      <c r="G28" t="n">
+        <v>270</v>
+      </c>
+      <c r="H28" t="n">
+        <v>135.1</v>
+      </c>
+      <c r="I28" t="n">
+        <v>63.3036</v>
+      </c>
+      <c r="J28" t="n">
+        <v>244</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1.0865107</v>
+      </c>
+      <c r="L28" t="n">
+        <v>5.606</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.4632517</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.3983274</v>
+      </c>
+      <c r="O28" t="n">
+        <v>7.3e-05</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>28</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1400</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.052262</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F29" t="n">
+        <v>233.6176</v>
+      </c>
+      <c r="G29" t="n">
+        <v>280</v>
+      </c>
+      <c r="H29" t="n">
+        <v>140.1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>65.0928</v>
+      </c>
+      <c r="J29" t="n">
+        <v>248</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1.1249652</v>
+      </c>
+      <c r="L29" t="n">
+        <v>5.608</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.4855237999999999</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.4134776999999999</v>
+      </c>
+      <c r="O29" t="n">
+        <v>7.7e-05</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>29</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1450</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.054312</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F30" t="n">
+        <v>242.9223</v>
+      </c>
+      <c r="G30" t="n">
+        <v>290</v>
+      </c>
+      <c r="H30" t="n">
+        <v>145.1</v>
+      </c>
+      <c r="I30" t="n">
+        <v>67.68680000000001</v>
+      </c>
+      <c r="J30" t="n">
+        <v>252</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1.1722159</v>
+      </c>
+      <c r="L30" t="n">
+        <v>5.61</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.4949288</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.4220791</v>
+      </c>
+      <c r="O30" t="n">
+        <v>7.499999999999999e-05</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.053527</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F31" t="n">
+        <v>251.8284</v>
+      </c>
+      <c r="G31" t="n">
+        <v>300</v>
+      </c>
+      <c r="H31" t="n">
+        <v>150.1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>70.50490000000001</v>
+      </c>
+      <c r="J31" t="n">
+        <v>256</v>
+      </c>
+      <c r="K31" t="n">
+        <v>1.249836</v>
+      </c>
+      <c r="L31" t="n">
+        <v>5.612</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.5251457</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.444462</v>
+      </c>
+      <c r="O31" t="n">
+        <v>8.3e-05</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>31</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1550</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.053991</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F32" t="n">
+        <v>264.1601000000001</v>
+      </c>
+      <c r="G32" t="n">
+        <v>310</v>
+      </c>
+      <c r="H32" t="n">
+        <v>155.1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>74.3873</v>
+      </c>
+      <c r="J32" t="n">
+        <v>260</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1.2422239</v>
+      </c>
+      <c r="L32" t="n">
+        <v>5.614</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.5199206999999999</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.4393398999999999</v>
+      </c>
+      <c r="O32" t="n">
+        <v>7.499999999999999e-05</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>32</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1600</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.052047</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F33" t="n">
+        <v>268.4022</v>
+      </c>
+      <c r="G33" t="n">
+        <v>320</v>
+      </c>
+      <c r="H33" t="n">
+        <v>160.1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>75.07730000000001</v>
+      </c>
+      <c r="J33" t="n">
+        <v>264</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1.2901004</v>
+      </c>
+      <c r="L33" t="n">
+        <v>5.616</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.5367636000000001</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.447736</v>
+      </c>
+      <c r="O33" t="n">
+        <v>8.3e-05</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1650</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.053405</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F34" t="n">
+        <v>276.7686</v>
+      </c>
+      <c r="G34" t="n">
+        <v>330</v>
+      </c>
+      <c r="H34" t="n">
+        <v>165.1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>77.57899999999999</v>
+      </c>
+      <c r="J34" t="n">
+        <v>268</v>
+      </c>
+      <c r="K34" t="n">
+        <v>1.3144532</v>
+      </c>
+      <c r="L34" t="n">
+        <v>5.618</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.5469216</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.4590264000000001</v>
+      </c>
+      <c r="O34" t="n">
+        <v>7.8e-05</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>34</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1700</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.05235</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F35" t="n">
+        <v>284.3133</v>
+      </c>
+      <c r="G35" t="n">
+        <v>340</v>
+      </c>
+      <c r="H35" t="n">
+        <v>170.1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>79.6896</v>
+      </c>
+      <c r="J35" t="n">
+        <v>272</v>
+      </c>
+      <c r="K35" t="n">
+        <v>1.3508602</v>
+      </c>
+      <c r="L35" t="n">
+        <v>5.62</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.5535213999999999</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.4588</v>
+      </c>
+      <c r="O35" t="n">
+        <v>7.9e-05</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>35</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1750</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.051268</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F36" t="n">
+        <v>287.0718</v>
+      </c>
+      <c r="G36" t="n">
+        <v>350</v>
+      </c>
+      <c r="H36" t="n">
+        <v>175.1</v>
+      </c>
+      <c r="I36" t="n">
+        <v>81.4665</v>
+      </c>
+      <c r="J36" t="n">
+        <v>276</v>
+      </c>
+      <c r="K36" t="n">
+        <v>1.3784345</v>
+      </c>
+      <c r="L36" t="n">
+        <v>5.622</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.5674713</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0.4683612</v>
+      </c>
+      <c r="O36" t="n">
+        <v>7.7e-05</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>36</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.051388</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F37" t="n">
+        <v>295.2204</v>
+      </c>
+      <c r="G37" t="n">
+        <v>360</v>
+      </c>
+      <c r="H37" t="n">
+        <v>180.1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>84.4211</v>
+      </c>
+      <c r="J37" t="n">
+        <v>280</v>
+      </c>
+      <c r="K37" t="n">
+        <v>1.4087369</v>
+      </c>
+      <c r="L37" t="n">
+        <v>5.624</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.5812351</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0.4800153999999999</v>
+      </c>
+      <c r="O37" t="n">
+        <v>7.7e-05</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>37</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1850</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.051294</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F38" t="n">
+        <v>307.175</v>
+      </c>
+      <c r="G38" t="n">
+        <v>370</v>
+      </c>
+      <c r="H38" t="n">
+        <v>185.1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>86.28869999999999</v>
+      </c>
+      <c r="J38" t="n">
+        <v>284</v>
+      </c>
+      <c r="K38" t="n">
+        <v>1.4641079</v>
+      </c>
+      <c r="L38" t="n">
+        <v>5.626</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.6003396999999999</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0.4917242</v>
+      </c>
+      <c r="O38" t="n">
+        <v>7.6e-05</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>38</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1900</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.053312</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F39" t="n">
+        <v>315.9537999999999</v>
+      </c>
+      <c r="G39" t="n">
+        <v>380</v>
+      </c>
+      <c r="H39" t="n">
+        <v>190.1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>88.7894</v>
+      </c>
+      <c r="J39" t="n">
+        <v>288</v>
+      </c>
+      <c r="K39" t="n">
+        <v>1.5015472</v>
+      </c>
+      <c r="L39" t="n">
+        <v>5.628</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.6152103999999999</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0.5018520000000001</v>
+      </c>
+      <c r="O39" t="n">
+        <v>8.1e-05</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>39</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1950</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.051273</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F40" t="n">
+        <v>323.439</v>
+      </c>
+      <c r="G40" t="n">
+        <v>390</v>
+      </c>
+      <c r="H40" t="n">
+        <v>195.1</v>
+      </c>
+      <c r="I40" t="n">
+        <v>91.801</v>
+      </c>
+      <c r="J40" t="n">
+        <v>292</v>
+      </c>
+      <c r="K40" t="n">
+        <v>1.5400794</v>
+      </c>
+      <c r="L40" t="n">
+        <v>5.63</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.6286948000000001</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0.511354</v>
+      </c>
+      <c r="O40" t="n">
+        <v>8.2e-05</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>40</v>
+      </c>
+      <c r="C41" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.051516</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1390</v>
+      </c>
+      <c r="F41" t="n">
+        <v>332.7085</v>
+      </c>
+      <c r="G41" t="n">
+        <v>400</v>
+      </c>
+      <c r="H41" t="n">
+        <v>200.1</v>
+      </c>
+      <c r="I41" t="n">
+        <v>93.64459999999998</v>
+      </c>
+      <c r="J41" t="n">
+        <v>296</v>
+      </c>
+      <c r="K41" t="n">
+        <v>1.5763463</v>
+      </c>
+      <c r="L41" t="n">
+        <v>5.632</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.6652976</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0.5457569</v>
+      </c>
+      <c r="O41" t="n">
+        <v>8.7e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>